<commit_message>
Accreditamento Winsap cs Anatomia Patologica #2
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap_CS
subject_application_version: 20.18.08
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.18.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_CS/20.18.00/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/CS_SESSIONE_20250317/Winsap_CS/20.18.00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{793048FF-51A5-4816-AEC5-7F1B97153AA6}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{6BB359D7-4C82-4617-8601-D4CF5A40298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67EED1A-0A0D-43BB-8D01-6850777776D3}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="475">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3897,10 +3897,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="N150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H181" sqref="H181"/>
+      <selection pane="bottomRight" activeCell="A155" sqref="A155:XFD155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -9634,7 +9634,9 @@
       <c r="G155" s="33"/>
       <c r="H155" s="33"/>
       <c r="I155" s="39"/>
-      <c r="J155" s="29"/>
+      <c r="J155" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="K155" s="29"/>
       <c r="L155" s="29"/>
       <c r="M155" s="29" t="s">
@@ -17576,6 +17578,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A6B8B41AB45FE4E8B23889C5F604192" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="c6632d705a2655bc4ef003303aa3e89d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="228e3216-9b37-47f7-9d85-6e6726edc181" xmlns:ns3="1e0ec522-3181-4f7c-b363-2ace71f6fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc3f6e4344a62cf01cb5a4907fa5259c" ns2:_="" ns3:_="">
     <xsd:import namespace="228e3216-9b37-47f7-9d85-6e6726edc181"/>
@@ -17770,27 +17792,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEDAFC9B-199E-4C7C-A64D-490A84C3B726}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17807,31 +17836,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>